<commit_message>
DEBUG: push exchange event into timeline
</commit_message>
<xml_diff>
--- a/basketBallRecorder/spreadsheet_for_timeLine.xlsx
+++ b/basketBallRecorder/spreadsheet_for_timeLine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27021"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="360" windowWidth="25600" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="6640" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>第一節</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,6 +58,66 @@
   </si>
   <si>
     <t>第四節</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延長賽一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>進攻方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延長賽二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>進攻方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出手方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>結果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延長賽三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延長賽四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>進攻方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出手方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罰球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延長賽五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>延長賽六</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -457,15 +517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:CA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:79">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,6 +608,132 @@
         <v>5</v>
       </c>
       <c r="AE1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>5</v>
+      </c>
+      <c r="CA1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add time to theevent in timeline xlsx
</commit_message>
<xml_diff>
--- a/basketBallRecorder/spreadsheet_for_timeLine.xlsx
+++ b/basketBallRecorder/spreadsheet_for_timeLine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27021"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>